<commit_message>
Version w/o pen up/down. ECE, but the C is weird
</commit_message>
<xml_diff>
--- a/angle_data.xlsx
+++ b/angle_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divija/Divi Drive/workplace/Princeton/Sem 5/Carlab/carlab_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277ABC1D-E563-7D43-B26D-7B1988BFD4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5B1C53-45A9-7C43-B69F-DB1ACAF6FE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{DCAFA70D-7DC0-C248-82D1-ACFBA3F5AF68}"/>
   </bookViews>
@@ -16,13 +16,13 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$X$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$X$2:$X$169</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$X$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$X$2:$X$169</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$AJ$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$AJ$2:$AJ$134</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$AJ$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$AJ$2:$AJ$134</definedName>
     <definedName name="theta_log" localSheetId="0">Sheet1!$A$1:$A$88</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{FE566A4F-80B2-C04A-A424-93AA92300BAD}" name="theta_log" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/divija/Divi Drive/workplace/Princeton/Sem 5/Carlab/carlab_2025/theta_log.csv">
+    <textPr sourceFile="/Users/divija/Divi Drive/workplace/Princeton/Sem 5/Carlab/carlab_2025/theta_log.csv">
       <textFields>
         <textField/>
       </textFields>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="1438">
   <si>
     <t>theta</t>
   </si>
@@ -5051,6 +5051,686 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="423454704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>theta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AJ$2:$AJ$134</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="133"/>
+                <c:pt idx="0">
+                  <c:v>0.66257121082900605</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62615660460599198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.46764393506436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4667668512143199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62556432085564095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56253313100700297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2916267052923498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55152437023532797</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.35666682767438102</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51882276732267996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.23105306363705</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.2669958874768501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.2489738415675899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.165263373258</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.471151895164441</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.36211532790977</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.45195526564548699</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.41031959504201</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.3940830527708901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.46819676040909</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-2.3458646423592802</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-2.33407882571891</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-2.37417023569764</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2.4164912004789398</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.2638871638411699</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.3002875665499398</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.1558061137513</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.9190663012503597</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.9418494669651798</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-5.0533194582994101</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-5.9580548296218101</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-5.1030927396011201</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-4.2679189061823903</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-3.3496250455846801</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-4.2236935629514196</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-2.5461498001013401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-2.4602345602323399</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6864081729092499</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.74001082140955</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.88613370262926106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.833394486525047</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.72977932504300302</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.72684487634572303</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.74064972507286397</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.134101237216461</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.107620410086014</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.72441206253571699</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.0327886342344199</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1.05156353210872</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.97865578598727299</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1.0697055674290199</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-2.73475070668507</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-3.48579148616684</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-3.5751962841198002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2.7052633768150298</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-3.6220874327689301</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-3.6588886497892101</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-3.5805363294200898</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-3.6617911756658801</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-3.67989052021791</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-4.4060907063635204</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-3.6319464786747599</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-3.71555751669875</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-2.7970747757283201</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-2.8192595770970899</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-2.14879312025987</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-2.9060002762543</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.2713732492265899</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0296668153777999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.6275877037009101</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.3744472236460998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1506855626776202</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.3837079458899999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.1681941026485401</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.1181972734805701</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.5048047366170998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.89980826326224395</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.71360257745418398</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-2.1562002291487299</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-4.5711820239694401</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-5.3622548093164903</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-6.2651947541625201</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-7.6851624338536997</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-8.5955379277862303</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-8.5864861291265804</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-8.6039589014942894</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-8.5820086131292292</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-7.6901656355341803</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-6.1667546489002296</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-4.6498414523062799</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-2.2841007429097302</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.0364799349836096E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.3160301902389202</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.3255097744009099</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.8321649641631499</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.6194470906656804</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.5893368706240203</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.5950099785187399</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.3704083572915904</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4.59114729196674</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4.5264496902663298</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.98461320991838</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.9659790655943898</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-0.13534384665310401</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-0.117437174526629</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-1.6378400038584999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-3.9358461372035798</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-4.7028490205787303</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-6.2301413401923398</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-8.4764702134170502</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-8.6929181380130505</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-9.3834055494395603</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-10.1488196409057</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-10.770967359879901</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-10.0064009898789</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-8.5566814674746698</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-6.9523990241809299</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-4.9179943616435002</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-1.8668319211639199</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.9076060896095</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.6273532108583399</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>7.0652416638085702</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9.9700395150782395</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>12.380947591321901</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>16.171618061002601</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>18.2858686902076</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>20.558765357874101</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>20.8140986288428</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>21.509228105309798</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>21.281420428866099</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>19.162065709749498</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>14.267410355998599</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>8.3063274308735302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FF5-A94E-8D26-1321D8E9C41A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1394530144"/>
+        <c:axId val="1394057664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1394530144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394057664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1394057664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394530144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10612,6 +11292,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -11487,6 +12207,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -15941,6 +17177,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>502478</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>64052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>104913</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>175224</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6ADCCE2-139E-CF79-99B1-C6CF7E94D54F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16265,10 +17537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9542BDE5-BFF2-C749-A1EE-9CD9BF57CBA1}">
-  <dimension ref="A1:AF1446"/>
+  <dimension ref="A1:AJ1446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AF1446"/>
+    <sheetView tabSelected="1" topLeftCell="X94" zoomScale="108" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="AP115" sqref="AP115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16276,7 +17548,7 @@
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16307,8 +17579,11 @@
       <c r="AF1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2.6358868853183899</v>
       </c>
@@ -16339,8 +17614,11 @@
       <c r="AF2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ2">
+        <v>0.66257121082900605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2.6670855521850498</v>
       </c>
@@ -16371,8 +17649,11 @@
       <c r="AF3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ3">
+        <v>0.62615660460599198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2.62978344942933</v>
       </c>
@@ -16403,8 +17684,11 @@
       <c r="AF4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ4">
+        <v>1.46764393506436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.64726418756646</v>
       </c>
@@ -16435,8 +17719,11 @@
       <c r="AF5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ5">
+        <v>1.4667668512143199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2.6510762087822601</v>
       </c>
@@ -16467,8 +17754,11 @@
       <c r="AF6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ6">
+        <v>0.62556432085564095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.81887024244845</v>
       </c>
@@ -16499,8 +17789,11 @@
       <c r="AF7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ7">
+        <v>0.56253313100700297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3.4464380963314998</v>
       </c>
@@ -16531,8 +17824,11 @@
       <c r="AF8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ8">
+        <v>2.2916267052923498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3.4588242108874798</v>
       </c>
@@ -16563,8 +17859,11 @@
       <c r="AF9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ9">
+        <v>0.55152437023532797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3.46116463055704</v>
       </c>
@@ -16595,8 +17894,11 @@
       <c r="AF10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ10">
+        <v>-0.35666682767438102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2.6293052671732</v>
       </c>
@@ -16627,8 +17929,11 @@
       <c r="AF11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ11">
+        <v>0.51882276732267996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.77135011437015</v>
       </c>
@@ -16659,8 +17964,11 @@
       <c r="AF12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ12">
+        <v>-1.23105306363705</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2.6129663102571001</v>
       </c>
@@ -16691,8 +17999,11 @@
       <c r="AF13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ13">
+        <v>-1.2669958874768501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2.59679922438669</v>
       </c>
@@ -16723,8 +18034,11 @@
       <c r="AF14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ14">
+        <v>-1.2489738415675899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.7491973104712699</v>
       </c>
@@ -16755,8 +18069,11 @@
       <c r="AF15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ15">
+        <v>-2.165263373258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2.5823116301032898</v>
       </c>
@@ -16787,8 +18104,11 @@
       <c r="AF16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ16">
+        <v>-0.471151895164441</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2.5739440063396199</v>
       </c>
@@ -16819,8 +18139,11 @@
       <c r="AF17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ17">
+        <v>-1.36211532790977</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2.5605030000629201</v>
       </c>
@@ -16851,8 +18174,11 @@
       <c r="AF18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ18">
+        <v>-0.45195526564548699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.7215894297116301</v>
       </c>
@@ -16883,8 +18209,11 @@
       <c r="AF19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ19">
+        <v>-1.41031959504201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2.5470302854278799</v>
       </c>
@@ -16915,8 +18244,11 @@
       <c r="AF20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ20">
+        <v>-2.3940830527708901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2.5376736832311599</v>
       </c>
@@ -16947,8 +18279,11 @@
       <c r="AF21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ21">
+        <v>-1.46819676040909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2.5283299504169499</v>
       </c>
@@ -16979,8 +18314,11 @@
       <c r="AF22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ22">
+        <v>-2.3458646423592802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2.5195818657615701</v>
       </c>
@@ -17011,8 +18349,11 @@
       <c r="AF23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ23">
+        <v>-2.33407882571891</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.6657333571430899</v>
       </c>
@@ -17043,8 +18384,11 @@
       <c r="AF24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ24">
+        <v>-2.37417023569764</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.82903028491958697</v>
       </c>
@@ -17075,8 +18419,11 @@
       <c r="AF25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ25">
+        <v>-2.4164912004789398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1.6372649953432701</v>
       </c>
@@ -17107,8 +18454,11 @@
       <c r="AF26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ26">
+        <v>-3.2638871638411699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.79752817475520899</v>
       </c>
@@ -17139,8 +18489,11 @@
       <c r="AF27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ27">
+        <v>-3.3002875665499398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1.6241950109679799</v>
       </c>
@@ -17171,8 +18524,11 @@
       <c r="AF28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ28">
+        <v>-4.1558061137513</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-2.1919740038151399E-2</v>
       </c>
@@ -17203,8 +18559,11 @@
       <c r="AF29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ29">
+        <v>-4.9190663012503597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-0.91874679381613999</v>
       </c>
@@ -17235,8 +18594,11 @@
       <c r="AF30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ30">
+        <v>-4.9418494669651798</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-1.6722223377940599</v>
       </c>
@@ -17267,8 +18629,11 @@
       <c r="AF31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ31">
+        <v>-5.0533194582994101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-1.77325628111603</v>
       </c>
@@ -17299,8 +18664,11 @@
       <c r="AF32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ32">
+        <v>-5.9580548296218101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-1.7849619208562799</v>
       </c>
@@ -17331,8 +18699,11 @@
       <c r="AF33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ33">
+        <v>-5.1030927396011201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-2.61660366414797</v>
       </c>
@@ -17363,8 +18734,11 @@
       <c r="AF34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ34">
+        <v>-4.2679189061823903</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-1.7841311677160101</v>
       </c>
@@ -17395,8 +18769,11 @@
       <c r="AF35" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ35">
+        <v>-3.3496250455846801</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-2.6142253276062699</v>
       </c>
@@ -17427,8 +18804,11 @@
       <c r="AF36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ36">
+        <v>-4.2236935629514196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-2.6192304030745102</v>
       </c>
@@ -17459,8 +18839,11 @@
       <c r="AF37" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ37">
+        <v>-2.5461498001013401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-2.5637612177614399</v>
       </c>
@@ -17491,8 +18874,11 @@
       <c r="AF38" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ38">
+        <v>-2.4602345602323399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-2.62674744727898</v>
       </c>
@@ -17523,8 +18909,11 @@
       <c r="AF39" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ39">
+        <v>-1.6864081729092499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-4.1924467662546503</v>
       </c>
@@ -17555,8 +18944,11 @@
       <c r="AF40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ40">
+        <v>-1.74001082140955</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>-4.1961322023198999</v>
       </c>
@@ -17587,8 +18979,11 @@
       <c r="AF41" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ41">
+        <v>-0.88613370262926106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-5.0959791775453098</v>
       </c>
@@ -17619,8 +19014,11 @@
       <c r="AF42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ42">
+        <v>-0.833394486525047</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-5.0073671790575602</v>
       </c>
@@ -17651,8 +19049,11 @@
       <c r="AF43" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ43">
+        <v>0.72977932504300302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-5.7501395205063499</v>
       </c>
@@ -17683,8 +19084,11 @@
       <c r="AF44" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ44">
+        <v>0.72684487634572303</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-5.8528161406784598</v>
       </c>
@@ -17715,8 +19119,11 @@
       <c r="AF45" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ45">
+        <v>0.74064972507286397</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-5.8569590208472802</v>
       </c>
@@ -17747,8 +19154,11 @@
       <c r="AF46" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ46">
+        <v>-0.134101237216461</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-5.8590448091302898</v>
       </c>
@@ -17779,8 +19189,11 @@
       <c r="AF47" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ47">
+        <v>-0.107620410086014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-6.6726738919567303</v>
       </c>
@@ -17811,8 +19224,11 @@
       <c r="AF48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ48">
+        <v>0.72441206253571699</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-7.6101996732628399</v>
       </c>
@@ -17843,8 +19259,11 @@
       <c r="AF49" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ49">
+        <v>-1.0327886342344199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-8.1723081638525592</v>
       </c>
@@ -17875,8 +19294,11 @@
       <c r="AF50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ50">
+        <v>-1.05156353210872</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-8.4668085985456898</v>
       </c>
@@ -17907,8 +19329,11 @@
       <c r="AF51" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ51">
+        <v>-0.97865578598727299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-8.9805532072098195</v>
       </c>
@@ -17939,8 +19364,11 @@
       <c r="AF52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ52">
+        <v>-1.0697055674290199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-7.5283097351191097</v>
       </c>
@@ -17971,8 +19399,11 @@
       <c r="AF53" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ53">
+        <v>-2.73475070668507</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-8.3303633755440192</v>
       </c>
@@ -18003,8 +19434,11 @@
       <c r="AF54" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ54">
+        <v>-3.48579148616684</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-9.0934452200217102</v>
       </c>
@@ -18035,8 +19469,11 @@
       <c r="AF55" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ55">
+        <v>-3.5751962841198002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-9.1253922111021808</v>
       </c>
@@ -18067,8 +19504,11 @@
       <c r="AF56" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ56">
+        <v>-2.7052633768150298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-10.7067203113397</v>
       </c>
@@ -18099,8 +19539,11 @@
       <c r="AF57" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ57">
+        <v>-3.6220874327689301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-10.718146975294999</v>
       </c>
@@ -18131,8 +19574,11 @@
       <c r="AF58" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ58">
+        <v>-3.6588886497892101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-10.891907154326301</v>
       </c>
@@ -18163,8 +19609,11 @@
       <c r="AF59" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ59">
+        <v>-3.5805363294200898</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-9.9233083446942096</v>
       </c>
@@ -18195,8 +19644,11 @@
       <c r="AF60" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ60">
+        <v>-3.6617911756658801</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-10.898951941894399</v>
       </c>
@@ -18227,8 +19679,11 @@
       <c r="AF61" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ61">
+        <v>-3.67989052021791</v>
+      </c>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-12.2661043668683</v>
       </c>
@@ -18259,8 +19714,11 @@
       <c r="AF62" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ62">
+        <v>-4.4060907063635204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-11.4922102108853</v>
       </c>
@@ -18291,8 +19749,11 @@
       <c r="AF63" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ63">
+        <v>-3.6319464786747599</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-10.713609084469001</v>
       </c>
@@ -18323,8 +19784,11 @@
       <c r="AF64" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ64">
+        <v>-3.71555751669875</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-10.7135275330946</v>
       </c>
@@ -18355,8 +19819,11 @@
       <c r="AF65" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ65">
+        <v>-2.7970747757283201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-10.713489436186601</v>
       </c>
@@ -18387,8 +19854,11 @@
       <c r="AF66" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ66">
+        <v>-2.8192595770970899</v>
+      </c>
+    </row>
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-12.268093452090699</v>
       </c>
@@ -18419,8 +19889,11 @@
       <c r="AF67" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ67">
+        <v>-2.14879312025987</v>
+      </c>
+    </row>
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-12.310506273621799</v>
       </c>
@@ -18451,8 +19924,11 @@
       <c r="AF68" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ68">
+        <v>-2.9060002762543</v>
+      </c>
+    </row>
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-13.0341766011648</v>
       </c>
@@ -18483,8 +19959,11 @@
       <c r="AF69" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ69">
+        <v>-1.2713732492265899</v>
+      </c>
+    </row>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-14.3432338112863</v>
       </c>
@@ -18515,8 +19994,11 @@
       <c r="AF70" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ70">
+        <v>1.0296668153777999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-14.5454485803493</v>
       </c>
@@ -18547,8 +20029,11 @@
       <c r="AF71" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ71">
+        <v>2.6275877037009101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-15.5155817521185</v>
       </c>
@@ -18579,8 +20064,11 @@
       <c r="AF72" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ72">
+        <v>3.3744472236460998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>-16.308223737388399</v>
       </c>
@@ -18611,8 +20099,11 @@
       <c r="AF73" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ73">
+        <v>4.1506855626776202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>-15.3199943648168</v>
       </c>
@@ -18643,8 +20134,11 @@
       <c r="AF74" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ74">
+        <v>3.3837079458899999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>-16.313999365078601</v>
       </c>
@@ -18675,8 +20169,11 @@
       <c r="AF75" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ75">
+        <v>4.1681941026485401</v>
+      </c>
+    </row>
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>-16.311270920415001</v>
       </c>
@@ -18707,8 +20204,11 @@
       <c r="AF76" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ76">
+        <v>4.1181972734805701</v>
+      </c>
+    </row>
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>-16.3082665481124</v>
       </c>
@@ -18739,8 +20239,11 @@
       <c r="AF77" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ77">
+        <v>2.5048047366170998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>-16.774936695904</v>
       </c>
@@ -18771,8 +20274,11 @@
       <c r="AF78" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ78">
+        <v>0.89980826326224395</v>
+      </c>
+    </row>
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>-16.771507575036001</v>
       </c>
@@ -18803,8 +20309,11 @@
       <c r="AF79" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ79">
+        <v>-0.71360257745418398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>-17.032163227994399</v>
       </c>
@@ -18835,8 +20344,11 @@
       <c r="AF80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ80">
+        <v>-2.1562002291487299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>-17.7686474419706</v>
       </c>
@@ -18867,8 +20379,11 @@
       <c r="AF81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ81">
+        <v>-4.5711820239694401</v>
+      </c>
+    </row>
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>-18.491180348257</v>
       </c>
@@ -18899,8 +20414,11 @@
       <c r="AF82" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ82">
+        <v>-5.3622548093164903</v>
+      </c>
+    </row>
+    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>-17.754840657080099</v>
       </c>
@@ -18931,8 +20449,11 @@
       <c r="AF83" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ83">
+        <v>-6.2651947541625201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>-17.721139185414</v>
       </c>
@@ -18963,8 +20484,11 @@
       <c r="AF84" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ84">
+        <v>-7.6851624338536997</v>
+      </c>
+    </row>
+    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>-19.895743970198598</v>
       </c>
@@ -18995,8 +20519,11 @@
       <c r="AF85" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ85">
+        <v>-8.5955379277862303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>-18.4727491263214</v>
       </c>
@@ -19027,8 +20554,11 @@
       <c r="AF86" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ86">
+        <v>-8.5864861291265804</v>
+      </c>
+    </row>
+    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>-19.448221448043299</v>
       </c>
@@ -19059,8 +20589,11 @@
       <c r="AF87" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ87">
+        <v>-8.6039589014942894</v>
+      </c>
+    </row>
+    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A88">
         <f>A55-10</f>
         <v>-19.09344522002171</v>
@@ -19092,8 +20625,11 @@
       <c r="AF88" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ88">
+        <v>-8.5820086131292292</v>
+      </c>
+    </row>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" ref="A89:A132" si="0">A56-10</f>
         <v>-19.125392211102181</v>
@@ -19125,8 +20661,11 @@
       <c r="AF89" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ89">
+        <v>-7.6901656355341803</v>
+      </c>
+    </row>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="0"/>
         <v>-20.706720311339701</v>
@@ -19158,8 +20697,11 @@
       <c r="AF90" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ90">
+        <v>-6.1667546489002296</v>
+      </c>
+    </row>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="0"/>
         <v>-20.718146975294999</v>
@@ -19191,8 +20733,11 @@
       <c r="AF91" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ91">
+        <v>-4.6498414523062799</v>
+      </c>
+    </row>
+    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="0"/>
         <v>-20.891907154326301</v>
@@ -19224,8 +20769,11 @@
       <c r="AF92" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ92">
+        <v>-2.2841007429097302</v>
+      </c>
+    </row>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="0"/>
         <v>-19.92330834469421</v>
@@ -19257,8 +20805,11 @@
       <c r="AF93" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ93">
+        <v>4.0364799349836096E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="0"/>
         <v>-20.898951941894399</v>
@@ -19290,8 +20841,11 @@
       <c r="AF94" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ94">
+        <v>2.3160301902389202</v>
+      </c>
+    </row>
+    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="0"/>
         <v>-22.266104366868298</v>
@@ -19323,8 +20877,11 @@
       <c r="AF95" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ95">
+        <v>2.3255097744009099</v>
+      </c>
+    </row>
+    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="0"/>
         <v>-21.4922102108853</v>
@@ -19356,8 +20913,11 @@
       <c r="AF96" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ96">
+        <v>3.8321649641631499</v>
+      </c>
+    </row>
+    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="0"/>
         <v>-20.713609084468999</v>
@@ -19389,8 +20949,11 @@
       <c r="AF97" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ97">
+        <v>4.6194470906656804</v>
+      </c>
+    </row>
+    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="0"/>
         <v>-20.713527533094599</v>
@@ -19422,8 +20985,11 @@
       <c r="AF98" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ98">
+        <v>4.5893368706240203</v>
+      </c>
+    </row>
+    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="0"/>
         <v>-20.713489436186599</v>
@@ -19452,8 +21018,11 @@
       <c r="AF99" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ99">
+        <v>4.5950099785187399</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="0"/>
         <v>-22.268093452090699</v>
@@ -19482,8 +21051,11 @@
       <c r="AF100" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ100">
+        <v>5.3704083572915904</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="0"/>
         <v>-22.310506273621797</v>
@@ -19512,8 +21084,11 @@
       <c r="AF101" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ101">
+        <v>4.59114729196674</v>
+      </c>
+    </row>
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="0"/>
         <v>-23.034176601164802</v>
@@ -19542,8 +21117,11 @@
       <c r="AF102" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ102">
+        <v>4.5264496902663298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="0"/>
         <v>-24.3432338112863</v>
@@ -19572,8 +21150,11 @@
       <c r="AF103" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ103">
+        <v>2.98461320991838</v>
+      </c>
+    </row>
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="0"/>
         <v>-24.545448580349301</v>
@@ -19602,8 +21183,11 @@
       <c r="AF104" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ104">
+        <v>2.9659790655943898</v>
+      </c>
+    </row>
+    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="0"/>
         <v>-25.5155817521185</v>
@@ -19632,8 +21216,11 @@
       <c r="AF105" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ105">
+        <v>-0.13534384665310401</v>
+      </c>
+    </row>
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="0"/>
         <v>-26.308223737388399</v>
@@ -19662,8 +21249,11 @@
       <c r="AF106" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ106">
+        <v>-0.117437174526629</v>
+      </c>
+    </row>
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="0"/>
         <v>-25.3199943648168</v>
@@ -19692,8 +21282,11 @@
       <c r="AF107" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ107">
+        <v>-1.6378400038584999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="0"/>
         <v>-26.313999365078601</v>
@@ -19722,8 +21315,11 @@
       <c r="AF108" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ108">
+        <v>-3.9358461372035798</v>
+      </c>
+    </row>
+    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="0"/>
         <v>-26.311270920415001</v>
@@ -19752,8 +21348,11 @@
       <c r="AF109" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ109">
+        <v>-4.7028490205787303</v>
+      </c>
+    </row>
+    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="0"/>
         <v>-26.3082665481124</v>
@@ -19782,8 +21381,11 @@
       <c r="AF110" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ110">
+        <v>-6.2301413401923398</v>
+      </c>
+    </row>
+    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="0"/>
         <v>-26.774936695904</v>
@@ -19812,8 +21414,11 @@
       <c r="AF111" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ111">
+        <v>-8.4764702134170502</v>
+      </c>
+    </row>
+    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="0"/>
         <v>-26.771507575036001</v>
@@ -19842,8 +21447,11 @@
       <c r="AF112" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ112">
+        <v>-8.6929181380130505</v>
+      </c>
+    </row>
+    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="0"/>
         <v>-27.032163227994399</v>
@@ -19872,8 +21480,11 @@
       <c r="AF113" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ113">
+        <v>-9.3834055494395603</v>
+      </c>
+    </row>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="0"/>
         <v>-27.7686474419706</v>
@@ -19902,8 +21513,11 @@
       <c r="AF114" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ114">
+        <v>-10.1488196409057</v>
+      </c>
+    </row>
+    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="0"/>
         <v>-28.491180348257</v>
@@ -19932,8 +21546,11 @@
       <c r="AF115" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ115">
+        <v>-10.770967359879901</v>
+      </c>
+    </row>
+    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="0"/>
         <v>-27.754840657080099</v>
@@ -19962,8 +21579,11 @@
       <c r="AF116" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ116">
+        <v>-10.0064009898789</v>
+      </c>
+    </row>
+    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="0"/>
         <v>-27.721139185414</v>
@@ -19992,8 +21612,11 @@
       <c r="AF117" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ117">
+        <v>-8.5566814674746698</v>
+      </c>
+    </row>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="0"/>
         <v>-29.895743970198598</v>
@@ -20022,8 +21645,11 @@
       <c r="AF118" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ118">
+        <v>-6.9523990241809299</v>
+      </c>
+    </row>
+    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="0"/>
         <v>-28.4727491263214</v>
@@ -20052,8 +21678,11 @@
       <c r="AF119" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ119">
+        <v>-4.9179943616435002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="0"/>
         <v>-29.448221448043299</v>
@@ -20082,8 +21711,11 @@
       <c r="AF120" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ120">
+        <v>-1.8668319211639199</v>
+      </c>
+    </row>
+    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A121">
         <f>A88-10</f>
         <v>-29.09344522002171</v>
@@ -20112,8 +21744,11 @@
       <c r="AF121" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ121">
+        <v>1.9076060896095</v>
+      </c>
+    </row>
+    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="0"/>
         <v>-29.125392211102181</v>
@@ -20142,8 +21777,11 @@
       <c r="AF122" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ122">
+        <v>2.6273532108583399</v>
+      </c>
+    </row>
+    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="0"/>
         <v>-30.706720311339701</v>
@@ -20172,8 +21810,11 @@
       <c r="AF123" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ123">
+        <v>7.0652416638085702</v>
+      </c>
+    </row>
+    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="0"/>
         <v>-30.718146975294999</v>
@@ -20202,8 +21843,11 @@
       <c r="AF124" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ124">
+        <v>9.9700395150782395</v>
+      </c>
+    </row>
+    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="0"/>
         <v>-30.891907154326301</v>
@@ -20232,8 +21876,11 @@
       <c r="AF125" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ125">
+        <v>12.380947591321901</v>
+      </c>
+    </row>
+    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="0"/>
         <v>-29.92330834469421</v>
@@ -20262,8 +21909,11 @@
       <c r="AF126" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ126">
+        <v>16.171618061002601</v>
+      </c>
+    </row>
+    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="0"/>
         <v>-30.898951941894399</v>
@@ -20292,8 +21942,11 @@
       <c r="AF127" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ127">
+        <v>18.2858686902076</v>
+      </c>
+    </row>
+    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="0"/>
         <v>-32.266104366868298</v>
@@ -20322,8 +21975,11 @@
       <c r="AF128" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ128">
+        <v>20.558765357874101</v>
+      </c>
+    </row>
+    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A129">
         <f>A96-10</f>
         <v>-31.4922102108853</v>
@@ -20352,8 +22008,11 @@
       <c r="AF129" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ129">
+        <v>20.8140986288428</v>
+      </c>
+    </row>
+    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="0"/>
         <v>-30.713609084468999</v>
@@ -20379,8 +22038,11 @@
       <c r="AF130" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ130">
+        <v>21.509228105309798</v>
+      </c>
+    </row>
+    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="0"/>
         <v>-30.713527533094599</v>
@@ -20406,8 +22068,11 @@
       <c r="AF131" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ131">
+        <v>21.281420428866099</v>
+      </c>
+    </row>
+    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="0"/>
         <v>-30.713489436186599</v>
@@ -20433,8 +22098,11 @@
       <c r="AF132" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ132">
+        <v>19.162065709749498</v>
+      </c>
+    </row>
+    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J133">
         <v>1.2678891450436001</v>
       </c>
@@ -20450,8 +22118,11 @@
       <c r="AF133" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ133">
+        <v>14.267410355998599</v>
+      </c>
+    </row>
+    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J134">
         <v>5.2475186963052796</v>
       </c>
@@ -20464,8 +22135,11 @@
       <c r="AF134" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AJ134">
+        <v>8.3063274308735302</v>
+      </c>
+    </row>
+    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J135">
         <v>8.3499482776934908</v>
       </c>
@@ -20479,7 +22153,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J136">
         <v>12.318542438114299</v>
       </c>
@@ -20493,7 +22167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J137">
         <v>14.762038138607901</v>
       </c>
@@ -20507,7 +22181,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J138">
         <v>15.5111664466255</v>
       </c>
@@ -20521,7 +22195,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="139" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
       <c r="J139">
         <v>17.973001090171401</v>
       </c>
@@ -20535,7 +22209,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
       <c r="L140">
         <v>-7.6843433830414503</v>
       </c>
@@ -20546,7 +22220,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
       <c r="L141">
         <v>-8.9861337587388999</v>
       </c>
@@ -20557,7 +22231,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
       <c r="L142">
         <v>-8.4064960574035901</v>
       </c>
@@ -20568,7 +22242,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
       <c r="L143">
         <v>-8.4213759743755201</v>
       </c>
@@ -20579,7 +22253,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
       <c r="L144">
         <v>-7.6865628822596301</v>
       </c>

</xml_diff>